<commit_message>
updated PAP to version 2
</commit_message>
<xml_diff>
--- a/variabellista.xlsx
+++ b/variabellista.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10204"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad.3103/Dropbox/Research/Education Choice - Spillovers and Returns/education_wealth/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E057347-F506-F742-B5F8-828B15D13DAB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="440" windowWidth="33600" windowHeight="20540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISA" sheetId="4" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="847">
   <si>
     <t>LISA</t>
   </si>
@@ -2237,6 +2238,354 @@
   </si>
   <si>
     <t>Födelsekvartal</t>
+  </si>
+  <si>
+    <t>Skollöpnummer</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Foreign background</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>yearly data</t>
+  </si>
+  <si>
+    <t>individual-unique data</t>
+  </si>
+  <si>
+    <t>degree year</t>
+  </si>
+  <si>
+    <t>education municipality</t>
+  </si>
+  <si>
+    <t>Municipality (living in)</t>
+  </si>
+  <si>
+    <t>source of data for highest edu</t>
+  </si>
+  <si>
+    <t>studying during the year</t>
+  </si>
+  <si>
+    <t>education group</t>
+  </si>
+  <si>
+    <t>education length</t>
+  </si>
+  <si>
+    <t>education field</t>
+  </si>
+  <si>
+    <t>study income (aid)</t>
+  </si>
+  <si>
+    <t>employment status</t>
+  </si>
+  <si>
+    <t>occupation SSYK-code</t>
+  </si>
+  <si>
+    <t>year for occupation data</t>
+  </si>
+  <si>
+    <t>wage</t>
+  </si>
+  <si>
+    <t>wage according to taxes</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>income net</t>
+  </si>
+  <si>
+    <t>consumption weight (family size)</t>
+  </si>
+  <si>
+    <t>disposable income</t>
+  </si>
+  <si>
+    <t>disposable income per consumption weight</t>
+  </si>
+  <si>
+    <t>connection adoptive parents</t>
+  </si>
+  <si>
+    <t>connection biological parents</t>
+  </si>
+  <si>
+    <t>connection siblings</t>
+  </si>
+  <si>
+    <t>income from largest source of income</t>
+  </si>
+  <si>
+    <t>data year</t>
+  </si>
+  <si>
+    <t>occupation data is the same as largest source of income</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>employer id</t>
+  </si>
+  <si>
+    <t>employer municipality</t>
+  </si>
+  <si>
+    <t>employer sector</t>
+  </si>
+  <si>
+    <t>employer sector other version</t>
+  </si>
+  <si>
+    <t>same for second largest income source</t>
+  </si>
+  <si>
+    <t>English - EDUCATION REGISTRY</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>course code</t>
+  </si>
+  <si>
+    <t>internal program code</t>
+  </si>
+  <si>
+    <t>scb program code</t>
+  </si>
+  <si>
+    <t>registered credits</t>
+  </si>
+  <si>
+    <t>finished credits</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>English - Elementary and High School</t>
+  </si>
+  <si>
+    <t>average grade</t>
+  </si>
+  <si>
+    <t>eligibility to university</t>
+  </si>
+  <si>
+    <t>gpa</t>
+  </si>
+  <si>
+    <t>school id</t>
+  </si>
+  <si>
+    <t>school municipality</t>
+  </si>
+  <si>
+    <t>school owner (public/private)</t>
+  </si>
+  <si>
+    <t>high school</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>graduation year</t>
+  </si>
+  <si>
+    <t>track code</t>
+  </si>
+  <si>
+    <t>public/private</t>
+  </si>
+  <si>
+    <t>high school 1997 -</t>
+  </si>
+  <si>
+    <t>grade document</t>
+  </si>
+  <si>
+    <t>eligibility</t>
+  </si>
+  <si>
+    <t>total nr credits</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>grades per course</t>
+  </si>
+  <si>
+    <t>centralized test in high school</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>grade in course</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test time</t>
+  </si>
+  <si>
+    <t>test result</t>
+  </si>
+  <si>
+    <t>Swedish SAT</t>
+  </si>
+  <si>
+    <t>normalized score</t>
+  </si>
+  <si>
+    <t>verbal score</t>
+  </si>
+  <si>
+    <t>quant score</t>
+  </si>
+  <si>
+    <t>raw scores verbal</t>
+  </si>
+  <si>
+    <t>raw scores quant</t>
+  </si>
+  <si>
+    <t>application data</t>
+  </si>
+  <si>
+    <t>Source 1 - UHR</t>
+  </si>
+  <si>
+    <t>year semester</t>
+  </si>
+  <si>
+    <t>application group</t>
+  </si>
+  <si>
+    <t>individual id</t>
+  </si>
+  <si>
+    <t>prio/ranking round 1</t>
+  </si>
+  <si>
+    <t>gpa round 1</t>
+  </si>
+  <si>
+    <t>queuenumber (admission result) round 1</t>
+  </si>
+  <si>
+    <t>tons of stuff over all kinds off applications for older data….</t>
+  </si>
+  <si>
+    <t>sum assets</t>
+  </si>
+  <si>
+    <t>sum debt</t>
+  </si>
+  <si>
+    <t>house market value</t>
+  </si>
+  <si>
+    <t>house tax value</t>
+  </si>
+  <si>
+    <t>farming property market value</t>
+  </si>
+  <si>
+    <t>summer house market value</t>
+  </si>
+  <si>
+    <t>tax value</t>
+  </si>
+  <si>
+    <t>rental house market value</t>
+  </si>
+  <si>
+    <t>industrial property market value</t>
+  </si>
+  <si>
+    <t>property abroad market value</t>
+  </si>
+  <si>
+    <t>owned apartment market value</t>
+  </si>
+  <si>
+    <t>bank account balance</t>
+  </si>
+  <si>
+    <t>bonds</t>
+  </si>
+  <si>
+    <t>bonds market value</t>
+  </si>
+  <si>
+    <t>mutual funds market value</t>
+  </si>
+  <si>
+    <t>stocks A -listed market value</t>
+  </si>
+  <si>
+    <t>stocks O -listed market value</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>insurance</t>
+  </si>
+  <si>
+    <t>other securities</t>
+  </si>
+  <si>
+    <t>other assets</t>
+  </si>
+  <si>
+    <t>total debt</t>
+  </si>
+  <si>
+    <t>study debt</t>
+  </si>
+  <si>
+    <t>total assets</t>
+  </si>
+  <si>
+    <t>financial assets</t>
+  </si>
+  <si>
+    <t>net assets market value</t>
+  </si>
+  <si>
+    <t>more detailed data on financial assets</t>
+  </si>
+  <si>
+    <t>wealth data (only available 1999-2007)</t>
   </si>
 </sst>
 </file>
@@ -2332,7 +2681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2376,6 +2725,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2396,6 +2748,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2712,10 +3067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2724,25 +3079,26 @@
     <col min="2" max="2" width="49.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2755,15 +3111,21 @@
       <c r="D3" s="4" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="F3" s="4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="F5" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>316</v>
       </c>
@@ -2772,7 +3134,7 @@
       </c>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>341</v>
       </c>
@@ -2781,13 +3143,13 @@
       </c>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>730</v>
       </c>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>342</v>
       </c>
@@ -2795,8 +3157,11 @@
         <v>347</v>
       </c>
       <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>343</v>
       </c>
@@ -2805,7 +3170,7 @@
       </c>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>344</v>
       </c>
@@ -2814,7 +3179,7 @@
       </c>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>345</v>
       </c>
@@ -2822,15 +3187,21 @@
         <v>350</v>
       </c>
       <c r="D12" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="F12" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="F14" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>339</v>
       </c>
@@ -2839,7 +3210,7 @@
       </c>
       <c r="D15" s="15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>357</v>
       </c>
@@ -2848,7 +3219,7 @@
       </c>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>363</v>
       </c>
@@ -2856,8 +3227,11 @@
         <v>363</v>
       </c>
       <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>355</v>
       </c>
@@ -2865,8 +3239,11 @@
         <v>356</v>
       </c>
       <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>390</v>
       </c>
@@ -2877,8 +3254,11 @@
         <v>409</v>
       </c>
       <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>362</v>
       </c>
@@ -2886,8 +3266,11 @@
         <v>395</v>
       </c>
       <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>371</v>
       </c>
@@ -2898,8 +3281,11 @@
         <v>410</v>
       </c>
       <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>375</v>
       </c>
@@ -2907,8 +3293,11 @@
         <v>407</v>
       </c>
       <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>376</v>
       </c>
@@ -2916,8 +3305,11 @@
         <v>408</v>
       </c>
       <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>405</v>
       </c>
@@ -2925,8 +3317,11 @@
         <v>406</v>
       </c>
       <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>369</v>
       </c>
@@ -2934,8 +3329,11 @@
         <v>370</v>
       </c>
       <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>373</v>
       </c>
@@ -2944,7 +3342,7 @@
       </c>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>377</v>
       </c>
@@ -2955,8 +3353,11 @@
         <v>420</v>
       </c>
       <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>389</v>
       </c>
@@ -2968,7 +3369,7 @@
       </c>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>384</v>
       </c>
@@ -2980,7 +3381,7 @@
       </c>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>411</v>
       </c>
@@ -2991,8 +3392,11 @@
         <v>413</v>
       </c>
       <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>414</v>
       </c>
@@ -3003,8 +3407,11 @@
         <v>413</v>
       </c>
       <c r="D31" s="15"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>416</v>
       </c>
@@ -3016,7 +3423,7 @@
       </c>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>417</v>
       </c>
@@ -3028,7 +3435,7 @@
       </c>
       <c r="D33" s="15"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>366</v>
       </c>
@@ -3036,8 +3443,11 @@
         <v>367</v>
       </c>
       <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>382</v>
       </c>
@@ -3049,7 +3459,7 @@
       </c>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>351</v>
       </c>
@@ -3060,8 +3470,11 @@
         <v>424</v>
       </c>
       <c r="D36" s="15"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>359</v>
       </c>
@@ -3069,8 +3482,11 @@
         <v>694</v>
       </c>
       <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>381</v>
       </c>
@@ -3081,8 +3497,11 @@
         <v>425</v>
       </c>
       <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>364</v>
       </c>
@@ -3090,8 +3509,11 @@
         <v>365</v>
       </c>
       <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>387</v>
       </c>
@@ -3100,7 +3522,7 @@
       </c>
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>353</v>
       </c>
@@ -3108,8 +3530,11 @@
         <v>354</v>
       </c>
       <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>386</v>
       </c>
@@ -3121,7 +3546,7 @@
       </c>
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>392</v>
       </c>
@@ -3129,8 +3554,11 @@
         <v>689</v>
       </c>
       <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>393</v>
       </c>
@@ -3142,17 +3570,20 @@
       </c>
       <c r="D44" s="15"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D45" s="15"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="21" t="s">
         <v>428</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="F46" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>316</v>
       </c>
@@ -3161,7 +3592,7 @@
       </c>
       <c r="D47" s="15"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>429</v>
       </c>
@@ -3170,7 +3601,7 @@
       </c>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>430</v>
       </c>
@@ -3179,14 +3610,17 @@
       </c>
       <c r="D49" s="15"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="20" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
         <v>433</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="F51" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>316</v>
       </c>
@@ -3195,7 +3629,7 @@
       </c>
       <c r="D52" s="15"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>429</v>
       </c>
@@ -3204,7 +3638,7 @@
       </c>
       <c r="D53" s="15"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>430</v>
       </c>
@@ -3213,14 +3647,17 @@
       </c>
       <c r="D54" s="15"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="21" t="s">
         <v>436</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="F56" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>316</v>
       </c>
@@ -3229,7 +3666,7 @@
       </c>
       <c r="D57" s="15"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>437</v>
       </c>
@@ -3238,7 +3675,7 @@
       </c>
       <c r="D58" s="15"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>438</v>
       </c>
@@ -3247,14 +3684,14 @@
       </c>
       <c r="D59" s="15"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="20" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -3267,8 +3704,11 @@
       <c r="D62" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F62" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>397</v>
       </c>
@@ -3281,8 +3721,11 @@
       <c r="D63" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F63" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>379</v>
       </c>
@@ -3295,8 +3738,11 @@
       <c r="D64" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F64" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>360</v>
       </c>
@@ -3310,7 +3756,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>399</v>
       </c>
@@ -3323,8 +3769,11 @@
       <c r="D66" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -3338,7 +3787,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -3351,8 +3800,11 @@
       <c r="D68" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3366,7 +3818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -3379,8 +3831,11 @@
       <c r="D70" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -3393,8 +3848,11 @@
       <c r="D71" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F71" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>15</v>
       </c>
@@ -3408,7 +3866,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -3422,7 +3880,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>21</v>
       </c>
@@ -3436,7 +3894,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -3450,7 +3908,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>25</v>
       </c>
@@ -3463,8 +3921,11 @@
       <c r="D76" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -3478,7 +3939,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -3492,7 +3953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>34</v>
       </c>
@@ -3506,18 +3967,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D80" s="15"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="20" t="s">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
       <c r="D81" s="15"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -3530,8 +3991,11 @@
       <c r="D82" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F82" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>401</v>
       </c>
@@ -3545,7 +4009,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>402</v>
       </c>
@@ -3559,7 +4023,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>403</v>
       </c>
@@ -3573,7 +4037,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>404</v>
       </c>
@@ -3587,7 +4051,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>38</v>
       </c>
@@ -3601,7 +4065,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -3615,7 +4079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>40</v>
       </c>
@@ -3629,7 +4093,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -3643,7 +4107,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -3657,7 +4121,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>43</v>
       </c>
@@ -3671,7 +4135,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>44</v>
       </c>
@@ -3685,7 +4149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -3699,7 +4163,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>46</v>
       </c>
@@ -3713,7 +4177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -3794,10 +4258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3805,23 +4269,24 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3834,16 +4299,19 @@
       <c r="D3" s="4" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="F3" s="4" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>441</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>316</v>
       </c>
@@ -3852,7 +4320,7 @@
       </c>
       <c r="D5" s="15"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>442</v>
       </c>
@@ -3860,8 +4328,11 @@
         <v>443</v>
       </c>
       <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>454</v>
       </c>
@@ -3869,8 +4340,11 @@
         <v>454</v>
       </c>
       <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>320</v>
       </c>
@@ -3878,8 +4352,11 @@
         <v>444</v>
       </c>
       <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>445</v>
       </c>
@@ -3888,7 +4365,7 @@
       </c>
       <c r="D9" s="15"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>447</v>
       </c>
@@ -3896,8 +4373,11 @@
         <v>448</v>
       </c>
       <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>449</v>
       </c>
@@ -3905,8 +4385,11 @@
         <v>450</v>
       </c>
       <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>451</v>
       </c>
@@ -3915,7 +4398,7 @@
       </c>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>455</v>
       </c>
@@ -3923,8 +4406,11 @@
         <v>458</v>
       </c>
       <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>452</v>
       </c>
@@ -3932,16 +4418,19 @@
         <v>453</v>
       </c>
       <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="F14" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>456</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -3951,7 +4440,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>442</v>
       </c>
@@ -3961,7 +4450,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>454</v>
       </c>
@@ -3971,7 +4460,7 @@
       <c r="C18" s="7"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>320</v>
       </c>
@@ -3981,7 +4470,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="15"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>445</v>
       </c>
@@ -3991,7 +4480,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>447</v>
       </c>
@@ -4001,7 +4490,7 @@
       <c r="C21" s="7"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>449</v>
       </c>
@@ -4011,7 +4500,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>451</v>
       </c>
@@ -4021,7 +4510,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>455</v>
       </c>
@@ -4031,7 +4520,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>452</v>
       </c>
@@ -4040,16 +4529,19 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="F25" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
         <v>466</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>320</v>
       </c>
@@ -4059,7 +4551,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>460</v>
       </c>
@@ -4069,7 +4561,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>462</v>
       </c>
@@ -4079,7 +4571,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>464</v>
       </c>
@@ -4087,11 +4579,14 @@
         <v>465</v>
       </c>
       <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>459</v>
       </c>
@@ -4114,10 +4609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F140"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4128,21 +4623,21 @@
     <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>467</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4155,16 +4650,19 @@
       <c r="D3" s="4" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="F3" s="4" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
         <v>505</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>316</v>
       </c>
@@ -4174,7 +4672,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="15"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>443</v>
       </c>
@@ -4184,7 +4682,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>468</v>
       </c>
@@ -4195,8 +4693,11 @@
         <v>509</v>
       </c>
       <c r="D8" s="15"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>470</v>
       </c>
@@ -4207,8 +4708,11 @@
         <v>508</v>
       </c>
       <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>471</v>
       </c>
@@ -4219,8 +4723,11 @@
         <v>508</v>
       </c>
       <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>506</v>
       </c>
@@ -4232,467 +4739,563 @@
       </c>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>731</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="19"/>
+      <c r="F12" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>727</v>
       </c>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D13" s="18"/>
+      <c r="F13" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>728</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>729</v>
       </c>
-      <c r="D13" s="18"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="D14" s="18"/>
+      <c r="F14" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>521</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B16" t="s">
-        <v>368</v>
-      </c>
-      <c r="D16" s="15"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="F16" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>481</v>
+        <v>316</v>
       </c>
       <c r="B17" t="s">
-        <v>481</v>
+        <v>368</v>
       </c>
       <c r="D17" s="15"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B18" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="D18" s="15"/>
+      <c r="F18" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B19" t="s">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="F19" s="7"/>
+      <c r="F19" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D20" s="15"/>
+      <c r="F20" s="7" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>727</v>
-      </c>
-      <c r="D21" s="18"/>
+        <v>480</v>
+      </c>
+      <c r="B21" t="s">
+        <v>485</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="F21" s="7" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>731</v>
+      </c>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>727</v>
+      </c>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>728</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>729</v>
       </c>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
+      <c r="D24" s="18"/>
+      <c r="F24" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
         <v>522</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>316</v>
-      </c>
-      <c r="B25" t="s">
-        <v>368</v>
-      </c>
-      <c r="D25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>486</v>
-      </c>
-      <c r="B26" t="s">
-        <v>487</v>
-      </c>
-      <c r="D26" s="15"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="F26" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>488</v>
+        <v>316</v>
       </c>
       <c r="B27" t="s">
-        <v>485</v>
+        <v>368</v>
       </c>
       <c r="D27" s="15"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="B28" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="D28" s="15"/>
+      <c r="F28" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B29" t="s">
-        <v>523</v>
+        <v>485</v>
       </c>
       <c r="D29" s="15"/>
+      <c r="F29" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B30" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D30" s="15"/>
+      <c r="F30" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D31" s="15"/>
+      <c r="F31" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>490</v>
+      </c>
+      <c r="B32" t="s">
+        <v>491</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="F32" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>492</v>
+      </c>
+      <c r="B33" t="s">
+        <v>524</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="F33" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>493</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>494</v>
       </c>
-      <c r="D32" s="15"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D34" s="15"/>
+      <c r="F34" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>495</v>
       </c>
-      <c r="D33" s="15"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>731</v>
+      </c>
+      <c r="D36" s="19"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>727</v>
       </c>
-      <c r="D34" s="18"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D37" s="18"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>728</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>729</v>
       </c>
-      <c r="D35" s="18"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+      <c r="D38" s="18"/>
+      <c r="F38" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="7"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="22" t="s">
         <v>496</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="F40" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>316</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>368</v>
       </c>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>497</v>
       </c>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>498</v>
       </c>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D43" s="15"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>483</v>
       </c>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>499</v>
       </c>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D45" s="15"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>500</v>
       </c>
-      <c r="D43" s="15"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D46" s="15"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>501</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>502</v>
       </c>
-      <c r="D44" s="15"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>483</v>
       </c>
-      <c r="D45" s="15"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>499</v>
       </c>
-      <c r="D46" s="15"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="D49" s="15"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>503</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="D47" s="15"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="D50" s="15"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>504</v>
       </c>
-      <c r="D48" s="15"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="21" t="s">
+      <c r="D51" s="15"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="F53" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>316</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B54" t="s">
         <v>368</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>442</v>
-      </c>
-      <c r="B52" t="s">
-        <v>443</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="D53" s="15"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>454</v>
-      </c>
-      <c r="B54" t="s">
-        <v>454</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="15"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>475</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>512</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>513</v>
-      </c>
+        <v>442</v>
+      </c>
+      <c r="B55" t="s">
+        <v>443</v>
+      </c>
+      <c r="C55" s="7"/>
       <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>476</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>514</v>
-      </c>
-      <c r="C56" s="7"/>
+      <c r="F55" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>517</v>
+      </c>
       <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>477</v>
+        <v>454</v>
       </c>
       <c r="B57" t="s">
-        <v>515</v>
+        <v>454</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>478</v>
-      </c>
-      <c r="B58" t="s">
-        <v>519</v>
-      </c>
-      <c r="C58" s="7"/>
+        <v>475</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>513</v>
+      </c>
       <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F58" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>479</v>
-      </c>
-      <c r="B59" t="s">
-        <v>520</v>
+        <v>476</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>514</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="15"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F59" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B60" t="s">
-        <v>516</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>513</v>
-      </c>
+        <v>515</v>
+      </c>
+      <c r="C60" s="7"/>
       <c r="D60" s="15"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F60" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>473</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>511</v>
+        <v>478</v>
+      </c>
+      <c r="B61" t="s">
+        <v>519</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="15"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="F61" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>479</v>
+      </c>
+      <c r="B62" t="s">
+        <v>520</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="15"/>
+      <c r="F62" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>480</v>
+      </c>
+      <c r="B63" t="s">
+        <v>516</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="D63" s="15"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>473</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="C64" s="7"/>
+      <c r="D64" s="15"/>
+      <c r="F64" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C63" s="7"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C64" s="7"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="7"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65" s="13"/>
+      <c r="D65" s="15"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C66" s="7"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C67" s="7"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68" s="7"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C69" s="7"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C70" s="7"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C71" s="7"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C72" s="7"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C73" s="7"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74" s="7"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C75" s="7"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" s="7"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" s="7"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78" s="7"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C79" s="7"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.2">
@@ -4875,14 +5478,23 @@
     <row r="140" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C140" s="7"/>
     </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C141" s="7"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C142" s="7"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C143" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A53:D53"/>
     <mergeCell ref="A1:D2"/>
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A40:D40"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4891,17 +5503,17 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="36" max="16383" man="1"/>
+    <brk id="39" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4912,21 +5524,21 @@
     <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>530</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -4939,8 +5551,11 @@
       <c r="D3" s="4" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -4952,7 +5567,7 @@
       </c>
       <c r="D4" s="15"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>443</v>
       </c>
@@ -4963,8 +5578,11 @@
         <v>700</v>
       </c>
       <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>525</v>
       </c>
@@ -4975,8 +5593,11 @@
         <v>700</v>
       </c>
       <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>531</v>
       </c>
@@ -4987,8 +5608,11 @@
         <v>700</v>
       </c>
       <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>526</v>
       </c>
@@ -4998,8 +5622,11 @@
       <c r="D8" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>527</v>
       </c>
@@ -5009,8 +5636,11 @@
       <c r="D9" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>528</v>
       </c>
@@ -5020,8 +5650,11 @@
       <c r="D10" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>529</v>
       </c>
@@ -5030,6 +5663,9 @@
       </c>
       <c r="D11" s="15" t="s">
         <v>57</v>
+      </c>
+      <c r="F11" t="s">
+        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -5049,8 +5685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5059,24 +5695,25 @@
     <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>617</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -5095,7 +5732,9 @@
         <v>698</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>810</v>
+      </c>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -5104,14 +5743,16 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>536</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="F5" s="12" t="s">
+        <v>811</v>
+      </c>
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -5125,6 +5766,9 @@
         <v>338</v>
       </c>
       <c r="D6" s="15"/>
+      <c r="F6" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -5137,6 +5781,9 @@
         <v>338</v>
       </c>
       <c r="D7" s="15"/>
+      <c r="F7" s="27" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -5149,6 +5796,9 @@
         <v>338</v>
       </c>
       <c r="D8" s="15"/>
+      <c r="F8" s="27" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -5161,6 +5811,9 @@
         <v>338</v>
       </c>
       <c r="D9" s="15"/>
+      <c r="F9" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -5173,6 +5826,9 @@
         <v>338</v>
       </c>
       <c r="D10" s="15"/>
+      <c r="F10" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -5185,6 +5841,9 @@
         <v>338</v>
       </c>
       <c r="D11" s="15"/>
+      <c r="F11" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -5197,6 +5856,9 @@
         <v>338</v>
       </c>
       <c r="D12" s="15"/>
+      <c r="F12" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -5209,6 +5871,9 @@
         <v>338</v>
       </c>
       <c r="D13" s="15"/>
+      <c r="F13" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -5221,6 +5886,9 @@
         <v>338</v>
       </c>
       <c r="D14" s="15"/>
+      <c r="F14" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -5246,7 +5914,7 @@
       </c>
       <c r="D16" s="15"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>334</v>
       </c>
@@ -5258,15 +5926,15 @@
       </c>
       <c r="D17" s="15"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
         <v>702</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>618</v>
       </c>
@@ -5279,8 +5947,11 @@
       <c r="D20" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>621</v>
       </c>
@@ -5293,8 +5964,11 @@
       <c r="D21" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>622</v>
       </c>
@@ -5308,7 +5982,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>537</v>
       </c>
@@ -5322,7 +5996,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>625</v>
       </c>
@@ -5336,7 +6010,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>627</v>
       </c>
@@ -5350,7 +6024,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>538</v>
       </c>
@@ -5364,7 +6038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>629</v>
       </c>
@@ -5378,7 +6052,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>631</v>
       </c>
@@ -5392,7 +6066,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>633</v>
       </c>
@@ -5406,7 +6080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>635</v>
       </c>
@@ -5420,7 +6094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>637</v>
       </c>
@@ -5434,7 +6108,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>639</v>
       </c>
@@ -5833,21 +6507,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>617</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -5875,12 +6549,12 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="21" t="s">
         <v>542</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -6333,10 +7007,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="103.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6344,16 +7018,17 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="113.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -6363,18 +7038,21 @@
       <c r="C2" s="4" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2" s="4" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>198</v>
       </c>
@@ -6384,8 +7062,11 @@
       <c r="C5" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>199</v>
       </c>
@@ -6395,18 +7076,21 @@
       <c r="C6" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>201</v>
       </c>
@@ -6416,8 +7100,11 @@
       <c r="C9" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>203</v>
       </c>
@@ -6427,8 +7114,11 @@
       <c r="C10" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>204</v>
       </c>
@@ -6438,8 +7128,11 @@
       <c r="C11" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>206</v>
       </c>
@@ -6450,7 +7143,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -6461,7 +7154,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>210</v>
       </c>
@@ -6472,7 +7165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>212</v>
       </c>
@@ -6482,8 +7175,11 @@
       <c r="C15" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>214</v>
       </c>
@@ -6493,8 +7189,11 @@
       <c r="C16" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>216</v>
       </c>
@@ -6505,7 +7204,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>218</v>
       </c>
@@ -6516,7 +7215,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>220</v>
       </c>
@@ -6527,7 +7226,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>222</v>
       </c>
@@ -6538,7 +7237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -6549,7 +7248,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>226</v>
       </c>
@@ -6559,8 +7258,11 @@
       <c r="C22" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>228</v>
       </c>
@@ -6571,7 +7273,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>230</v>
       </c>
@@ -6582,7 +7284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>232</v>
       </c>
@@ -6593,7 +7295,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>234</v>
       </c>
@@ -6604,7 +7306,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>236</v>
       </c>
@@ -6614,8 +7316,11 @@
       <c r="C27" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>238</v>
       </c>
@@ -6626,7 +7331,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>240</v>
       </c>
@@ -6637,7 +7342,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>242</v>
       </c>
@@ -6647,8 +7352,11 @@
       <c r="C30" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>244</v>
       </c>
@@ -6659,7 +7367,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>246</v>
       </c>
@@ -6670,7 +7378,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>248</v>
       </c>
@@ -6681,7 +7389,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>250</v>
       </c>
@@ -6692,7 +7400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>252</v>
       </c>
@@ -6703,7 +7411,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>254</v>
       </c>
@@ -6714,7 +7422,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>256</v>
       </c>
@@ -6725,7 +7433,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -6736,7 +7444,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>260</v>
       </c>
@@ -6746,8 +7454,11 @@
       <c r="C39" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -6758,17 +7469,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C41" s="17"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="20" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>64</v>
       </c>
@@ -6778,8 +7489,11 @@
       <c r="C43" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>262</v>
       </c>
@@ -6789,8 +7503,11 @@
       <c r="C44" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>263</v>
       </c>
@@ -6801,7 +7518,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>265</v>
       </c>
@@ -6811,8 +7528,11 @@
       <c r="C46" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>266</v>
       </c>
@@ -6823,7 +7543,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>267</v>
       </c>
@@ -6834,7 +7554,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>268</v>
       </c>
@@ -6845,7 +7565,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>269</v>
       </c>
@@ -6856,7 +7576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>270</v>
       </c>
@@ -6867,7 +7587,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>271</v>
       </c>
@@ -6877,8 +7597,11 @@
       <c r="C52" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>273</v>
       </c>
@@ -6889,7 +7612,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>275</v>
       </c>
@@ -6899,8 +7622,11 @@
       <c r="C54" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>277</v>
       </c>
@@ -6911,7 +7637,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>279</v>
       </c>
@@ -6922,7 +7648,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>281</v>
       </c>
@@ -6932,8 +7658,11 @@
       <c r="C57" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>283</v>
       </c>
@@ -6944,7 +7673,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>285</v>
       </c>
@@ -6954,8 +7683,11 @@
       <c r="C59" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>287</v>
       </c>
@@ -6965,8 +7697,11 @@
       <c r="C60" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>288</v>
       </c>
@@ -6977,7 +7712,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>158</v>
       </c>
@@ -6987,8 +7722,11 @@
       <c r="C62" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>156</v>
       </c>
@@ -6999,7 +7737,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>289</v>
       </c>
@@ -7010,7 +7748,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>291</v>
       </c>
@@ -7020,8 +7758,11 @@
       <c r="C65" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>293</v>
       </c>
@@ -7032,17 +7773,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C67" s="17"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="20" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>296</v>
       </c>
@@ -7052,8 +7793,11 @@
       <c r="C69" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E69" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>297</v>
       </c>
@@ -7064,17 +7808,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C71" s="17"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="20" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>94</v>
       </c>
@@ -7084,8 +7828,11 @@
       <c r="C73" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E73" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>300</v>
       </c>
@@ -7096,7 +7843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>302</v>
       </c>
@@ -7107,7 +7854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>303</v>
       </c>
@@ -7117,18 +7864,21 @@
       <c r="C76" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E76" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C77" s="17"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="20" t="s">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -7138,8 +7888,11 @@
       <c r="C79" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E79" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>308</v>
       </c>
@@ -7149,8 +7902,11 @@
       <c r="C80" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>310</v>
       </c>
@@ -7161,7 +7917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>312</v>
       </c>
@@ -7172,7 +7928,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>314</v>
       </c>
@@ -7182,20 +7938,23 @@
       <c r="C83" s="17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="22" t="s">
+      <c r="E83" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="B85" s="22"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="22" t="s">
+      <c r="B85" s="23"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="B86" s="22"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B86" s="23"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>690</v>
       </c>
@@ -7223,10 +7982,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K139"/>
+  <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7236,13 +7995,16 @@
     <col min="3" max="11" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>723</v>
       </c>
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" s="26"/>
+      <c r="M1" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C2" s="1">
         <v>1999</v>
       </c>
@@ -7271,11 +8033,11 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
@@ -7298,7 +8060,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -7306,7 +8068,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -7314,7 +8076,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -7322,7 +8084,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -7330,7 +8092,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -7338,11 +8100,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
         <v>725</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
@@ -7371,7 +8133,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -7379,7 +8141,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -7387,7 +8149,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -7395,7 +8157,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -7403,7 +8165,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -7468,10 +8230,10 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="24"/>
+      <c r="B25" s="25"/>
       <c r="C25" s="1" t="s">
         <v>57</v>
       </c>
@@ -7543,10 +8305,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="1" t="s">
         <v>57</v>
       </c>
@@ -7586,10 +8348,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="1" t="s">
         <v>57</v>
       </c>
@@ -7707,10 +8469,10 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B50" s="24"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="1" t="s">
         <v>57</v>
       </c>
@@ -7798,10 +8560,10 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="24"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="1" t="s">
         <v>57</v>
       </c>
@@ -7903,10 +8665,10 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="24"/>
+      <c r="B71" s="25"/>
       <c r="G71" s="1" t="s">
         <v>57</v>
       </c>
@@ -8004,10 +8766,10 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="24" t="s">
+      <c r="A83" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B83" s="24"/>
+      <c r="B83" s="25"/>
       <c r="G83" s="1" t="s">
         <v>57</v>
       </c>
@@ -8097,10 +8859,10 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="24" t="s">
+      <c r="A94" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="B94" s="24"/>
+      <c r="B94" s="25"/>
       <c r="C94" s="1" t="s">
         <v>57</v>
       </c>
@@ -8196,10 +8958,10 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="24" t="s">
+      <c r="A105" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="B105" s="24"/>
+      <c r="B105" s="25"/>
       <c r="C105" s="1" t="s">
         <v>57</v>
       </c>
@@ -8239,10 +9001,10 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A109" s="24" t="s">
+      <c r="A109" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="24"/>
+      <c r="B109" s="25"/>
       <c r="G109" s="1" t="s">
         <v>57</v>
       </c>
@@ -8284,10 +9046,10 @@
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" s="24" t="s">
+      <c r="A114" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="B114" s="24"/>
+      <c r="B114" s="25"/>
       <c r="C114" s="1" t="s">
         <v>57</v>
       </c>
@@ -8423,10 +9185,10 @@
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A130" s="24" t="s">
+      <c r="A130" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="B130" s="24"/>
+      <c r="B130" s="25"/>
       <c r="G130" s="1" t="s">
         <v>57</v>
       </c>
@@ -8460,10 +9222,10 @@
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A134" s="24" t="s">
+      <c r="A134" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="B134" s="24"/>
+      <c r="B134" s="25"/>
       <c r="G134" s="1" t="s">
         <v>57</v>
       </c>

</xml_diff>